<commit_message>
Updates to figures, add figure of overall productivity
Added histogram to mortality model, added figure showing plot-level proportion productivity
</commit_message>
<xml_diff>
--- a/Giselda_Data_per_plot.xlsx
+++ b/Giselda_Data_per_plot.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\Research\Assis tree growth\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C85B364-CE30-4961-9FDE-194A83C5ECDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9060"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data per plot" sheetId="6" r:id="rId1"/>
     <sheet name="Methods" sheetId="8" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519" iterate="1"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -100,13 +106,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="&quot;R$ &quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -602,25 +608,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="2"/>
+    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.7109375" customWidth="1"/>
     <col min="17" max="17" width="9.140625" style="2"/>
     <col min="18" max="18" width="11.140625" customWidth="1"/>
@@ -815,7 +822,7 @@
     <col min="16096" max="16096" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="60">
+    <row r="1" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>15</v>
       </c>
@@ -871,7 +878,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -927,7 +934,7 @@
         <v>0.30415331903880055</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -983,7 +990,7 @@
         <v>0.2883945323314529</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1039,7 +1046,7 @@
         <v>0.30955454237191155</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1095,7 +1102,7 @@
         <v>0.30618397045483853</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1151,7 +1158,7 @@
         <v>0.36332986183759791</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -1207,7 +1214,7 @@
         <v>0.27876049551872606</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1263,7 +1270,7 @@
         <v>0.29643968597089126</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -1319,7 +1326,7 @@
         <v>0.34319054711880004</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -1375,7 +1382,7 @@
         <v>0.31148261008647493</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -1431,7 +1438,7 @@
         <v>0.27544966268148241</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -1487,7 +1494,7 @@
         <v>0.33884984633848897</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -1543,7 +1550,7 @@
         <v>0.23473440236271931</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>13</v>
       </c>
@@ -1599,7 +1606,7 @@
         <v>0.31691370730417101</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>14</v>
       </c>
@@ -1655,7 +1662,7 @@
         <v>0.3751105787592956</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>15</v>
       </c>
@@ -1711,7 +1718,7 @@
         <v>0.28993656521914385</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>16</v>
       </c>
@@ -1767,7 +1774,7 @@
         <v>0.27952920455187552</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>17</v>
       </c>
@@ -1823,7 +1830,7 @@
         <v>0.26630074389998415</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>18</v>
       </c>
@@ -1879,7 +1886,7 @@
         <v>0.25748495778911473</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -1935,7 +1942,7 @@
         <v>0.30932166837153335</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -1991,7 +1998,7 @@
         <v>0.26087181801338016</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>26</v>
       </c>
@@ -2047,7 +2054,7 @@
         <v>0.20041887086129614</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>27</v>
       </c>
@@ -2103,7 +2110,7 @@
         <v>0.22640724933301326</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>28</v>
       </c>
@@ -2159,7 +2166,7 @@
         <v>0.16490399648128692</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>29</v>
       </c>
@@ -2215,7 +2222,7 @@
         <v>0.2138643269695415</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>30</v>
       </c>
@@ -2271,7 +2278,7 @@
         <v>0.19470047436462154</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>31</v>
       </c>
@@ -2327,7 +2334,7 @@
         <v>0.15836846731240253</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>32</v>
       </c>
@@ -2383,7 +2390,7 @@
         <v>0.18941278280092269</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>33</v>
       </c>
@@ -2439,7 +2446,7 @@
         <v>0.13630427299463896</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>34</v>
       </c>
@@ -2495,7 +2502,7 @@
         <v>0.1411699414914257</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>35</v>
       </c>
@@ -2551,407 +2558,407 @@
         <v>0.28258833095065866</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32" s="15"/>
       <c r="K32" s="17"/>
       <c r="R32" s="25"/>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
       <c r="K33" s="17"/>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="K34" s="17"/>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="K35" s="17"/>
       <c r="N35" s="10"/>
       <c r="O35" s="10"/>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="K36" s="17"/>
       <c r="N36" s="10"/>
       <c r="O36" s="10"/>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="K37" s="17"/>
       <c r="N37" s="10"/>
       <c r="O37" s="10"/>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="17"/>
       <c r="B38" s="18"/>
       <c r="K38" s="17"/>
       <c r="N38" s="10"/>
       <c r="O38" s="10"/>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K39" s="17"/>
       <c r="N39" s="10"/>
       <c r="O39" s="10"/>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K40" s="17"/>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K41" s="17"/>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K42" s="17"/>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K43" s="17"/>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K44" s="17"/>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K45" s="17"/>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K46" s="17"/>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K47" s="17"/>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K48" s="17"/>
     </row>
-    <row r="49" spans="11:11">
+    <row r="49" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K49" s="17"/>
     </row>
-    <row r="50" spans="11:11">
+    <row r="50" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K50" s="17"/>
     </row>
-    <row r="51" spans="11:11">
+    <row r="51" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K51" s="17"/>
     </row>
-    <row r="52" spans="11:11">
+    <row r="52" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K52" s="17"/>
     </row>
-    <row r="53" spans="11:11">
+    <row r="53" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K53" s="17"/>
     </row>
-    <row r="54" spans="11:11">
+    <row r="54" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K54" s="17"/>
     </row>
-    <row r="55" spans="11:11">
+    <row r="55" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K55" s="17"/>
     </row>
-    <row r="56" spans="11:11">
+    <row r="56" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K56" s="17"/>
     </row>
-    <row r="57" spans="11:11">
+    <row r="57" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K57" s="17"/>
     </row>
-    <row r="58" spans="11:11">
+    <row r="58" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K58" s="17"/>
     </row>
-    <row r="59" spans="11:11">
+    <row r="59" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K59" s="17"/>
     </row>
-    <row r="60" spans="11:11">
+    <row r="60" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K60" s="17"/>
     </row>
-    <row r="61" spans="11:11">
+    <row r="61" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K61" s="17"/>
     </row>
-    <row r="62" spans="11:11">
+    <row r="62" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K62" s="17"/>
     </row>
-    <row r="63" spans="11:11">
+    <row r="63" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K63" s="17"/>
     </row>
-    <row r="64" spans="11:11">
+    <row r="64" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K64" s="17"/>
     </row>
-    <row r="65" spans="11:11">
+    <row r="65" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K65" s="17"/>
     </row>
-    <row r="66" spans="11:11">
+    <row r="66" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K66" s="17"/>
     </row>
-    <row r="67" spans="11:11">
+    <row r="67" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K67" s="17"/>
     </row>
-    <row r="68" spans="11:11">
+    <row r="68" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K68" s="17"/>
     </row>
-    <row r="69" spans="11:11">
+    <row r="69" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K69" s="17"/>
     </row>
-    <row r="70" spans="11:11">
+    <row r="70" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K70" s="17"/>
     </row>
-    <row r="71" spans="11:11">
+    <row r="71" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K71" s="17"/>
     </row>
-    <row r="72" spans="11:11">
+    <row r="72" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K72" s="17"/>
     </row>
-    <row r="73" spans="11:11">
+    <row r="73" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K73" s="17"/>
     </row>
-    <row r="74" spans="11:11">
+    <row r="74" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K74" s="17"/>
     </row>
-    <row r="75" spans="11:11">
+    <row r="75" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K75" s="17"/>
     </row>
-    <row r="76" spans="11:11">
+    <row r="76" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K76" s="17"/>
     </row>
-    <row r="77" spans="11:11">
+    <row r="77" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K77" s="17"/>
     </row>
-    <row r="78" spans="11:11">
+    <row r="78" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K78" s="17"/>
     </row>
-    <row r="79" spans="11:11">
+    <row r="79" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K79" s="17"/>
     </row>
-    <row r="80" spans="11:11">
+    <row r="80" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K80" s="17"/>
     </row>
-    <row r="81" spans="11:11">
+    <row r="81" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K81" s="17"/>
     </row>
-    <row r="82" spans="11:11">
+    <row r="82" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K82" s="17"/>
     </row>
-    <row r="83" spans="11:11">
+    <row r="83" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K83" s="17"/>
     </row>
-    <row r="84" spans="11:11">
+    <row r="84" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K84" s="17"/>
     </row>
-    <row r="85" spans="11:11">
+    <row r="85" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K85" s="17"/>
     </row>
-    <row r="86" spans="11:11">
+    <row r="86" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K86" s="17"/>
     </row>
-    <row r="87" spans="11:11">
+    <row r="87" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K87" s="17"/>
     </row>
-    <row r="88" spans="11:11">
+    <row r="88" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K88" s="17"/>
     </row>
-    <row r="89" spans="11:11">
+    <row r="89" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K89" s="17"/>
     </row>
-    <row r="90" spans="11:11">
+    <row r="90" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K90" s="17"/>
     </row>
-    <row r="91" spans="11:11">
+    <row r="91" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K91" s="17"/>
     </row>
-    <row r="92" spans="11:11">
+    <row r="92" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K92" s="17"/>
     </row>
-    <row r="93" spans="11:11">
+    <row r="93" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K93" s="17"/>
     </row>
-    <row r="94" spans="11:11">
+    <row r="94" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K94" s="17"/>
     </row>
-    <row r="95" spans="11:11">
+    <row r="95" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K95" s="17"/>
     </row>
-    <row r="96" spans="11:11">
+    <row r="96" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K96" s="17"/>
     </row>
-    <row r="97" spans="11:11">
+    <row r="97" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K97" s="17"/>
     </row>
-    <row r="98" spans="11:11">
+    <row r="98" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K98" s="17"/>
     </row>
-    <row r="99" spans="11:11">
+    <row r="99" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K99" s="17"/>
     </row>
-    <row r="100" spans="11:11">
+    <row r="100" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K100" s="17"/>
     </row>
-    <row r="101" spans="11:11">
+    <row r="101" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K101" s="17"/>
     </row>
-    <row r="102" spans="11:11">
+    <row r="102" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K102" s="17"/>
     </row>
-    <row r="103" spans="11:11">
+    <row r="103" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K103" s="17"/>
     </row>
-    <row r="104" spans="11:11">
+    <row r="104" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K104" s="17"/>
     </row>
-    <row r="105" spans="11:11">
+    <row r="105" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K105" s="17"/>
     </row>
-    <row r="106" spans="11:11">
+    <row r="106" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K106" s="17"/>
     </row>
-    <row r="107" spans="11:11">
+    <row r="107" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K107" s="17"/>
     </row>
-    <row r="108" spans="11:11">
+    <row r="108" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K108" s="17"/>
     </row>
-    <row r="109" spans="11:11">
+    <row r="109" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K109" s="17"/>
     </row>
-    <row r="110" spans="11:11">
+    <row r="110" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K110" s="17"/>
     </row>
-    <row r="111" spans="11:11">
+    <row r="111" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K111" s="17"/>
     </row>
-    <row r="112" spans="11:11">
+    <row r="112" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K112" s="17"/>
     </row>
-    <row r="113" spans="11:11">
+    <row r="113" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K113" s="17"/>
     </row>
-    <row r="114" spans="11:11">
+    <row r="114" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K114" s="17"/>
     </row>
-    <row r="115" spans="11:11">
+    <row r="115" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K115" s="17"/>
     </row>
-    <row r="116" spans="11:11">
+    <row r="116" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K116" s="17"/>
     </row>
-    <row r="117" spans="11:11">
+    <row r="117" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K117" s="17"/>
     </row>
-    <row r="118" spans="11:11">
+    <row r="118" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K118" s="17"/>
     </row>
-    <row r="119" spans="11:11">
+    <row r="119" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K119" s="17"/>
     </row>
-    <row r="120" spans="11:11">
+    <row r="120" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K120" s="17"/>
     </row>
-    <row r="121" spans="11:11">
+    <row r="121" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K121" s="17"/>
     </row>
-    <row r="122" spans="11:11">
+    <row r="122" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K122" s="17"/>
     </row>
-    <row r="123" spans="11:11">
+    <row r="123" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K123" s="17"/>
     </row>
-    <row r="124" spans="11:11">
+    <row r="124" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K124" s="17"/>
     </row>
-    <row r="125" spans="11:11">
+    <row r="125" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K125" s="17"/>
     </row>
-    <row r="126" spans="11:11">
+    <row r="126" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K126" s="17"/>
     </row>
-    <row r="127" spans="11:11">
+    <row r="127" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K127" s="17"/>
     </row>
-    <row r="128" spans="11:11">
+    <row r="128" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K128" s="17"/>
     </row>
-    <row r="129" spans="11:11">
+    <row r="129" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K129" s="17"/>
     </row>
-    <row r="130" spans="11:11">
+    <row r="130" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K130" s="17"/>
     </row>
-    <row r="131" spans="11:11">
+    <row r="131" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K131" s="17"/>
     </row>
-    <row r="132" spans="11:11">
+    <row r="132" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K132" s="17"/>
     </row>
-    <row r="133" spans="11:11">
+    <row r="133" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K133" s="17"/>
     </row>
-    <row r="134" spans="11:11">
+    <row r="134" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K134" s="17"/>
     </row>
-    <row r="135" spans="11:11">
+    <row r="135" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K135" s="17"/>
     </row>
-    <row r="136" spans="11:11">
+    <row r="136" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K136" s="17"/>
     </row>
-    <row r="137" spans="11:11">
+    <row r="137" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K137" s="17"/>
     </row>
-    <row r="138" spans="11:11">
+    <row r="138" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K138" s="17"/>
     </row>
-    <row r="139" spans="11:11">
+    <row r="139" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K139" s="17"/>
     </row>
-    <row r="140" spans="11:11">
+    <row r="140" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K140" s="17"/>
     </row>
-    <row r="141" spans="11:11">
+    <row r="141" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K141" s="17"/>
     </row>
-    <row r="142" spans="11:11">
+    <row r="142" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K142" s="17"/>
     </row>
-    <row r="143" spans="11:11">
+    <row r="143" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K143" s="17"/>
     </row>
-    <row r="144" spans="11:11">
+    <row r="144" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K144" s="17"/>
     </row>
-    <row r="145" spans="11:11">
+    <row r="145" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K145" s="17"/>
     </row>
-    <row r="146" spans="11:11">
+    <row r="146" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K146" s="17"/>
     </row>
-    <row r="147" spans="11:11">
+    <row r="147" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K147" s="17"/>
     </row>
-    <row r="148" spans="11:11">
+    <row r="148" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K148" s="17"/>
     </row>
-    <row r="149" spans="11:11">
+    <row r="149" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K149" s="17"/>
     </row>
-    <row r="150" spans="11:11">
+    <row r="150" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K150" s="17"/>
     </row>
-    <row r="151" spans="11:11">
+    <row r="151" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K151" s="17"/>
     </row>
-    <row r="152" spans="11:11">
+    <row r="152" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K152" s="17"/>
     </row>
-    <row r="153" spans="11:11">
+    <row r="153" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K153" s="17"/>
     </row>
-    <row r="154" spans="11:11">
+    <row r="154" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K154" s="17"/>
     </row>
-    <row r="155" spans="11:11">
+    <row r="155" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K155" s="17"/>
     </row>
-    <row r="156" spans="11:11">
+    <row r="156" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K156" s="17"/>
     </row>
-    <row r="157" spans="11:11">
+    <row r="157" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K157" s="17"/>
     </row>
   </sheetData>
@@ -2960,46 +2967,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="21">
+    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="29" customFormat="1" ht="15.75">
+    <row r="2" spans="1:1" s="29" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>

</xml_diff>